<commit_message>
Sprint-1 Week-1 : Tests are marked for execution
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/DOCS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/DOCS Suite.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIWS\Falcrum_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>TCID</t>
   </si>
@@ -52,19 +52,12 @@
   </si>
   <si>
     <t>Sprint1</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -489,15 +482,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="73.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -533,9 +528,7 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Included and marked for execution -FLD_DocumentRegistry_New_Transmittals
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/DOCS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/DOCS Suite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TCID</t>
   </si>
@@ -45,13 +45,16 @@
     <t>N</t>
   </si>
   <si>
-    <t>Documents_New</t>
-  </si>
-  <si>
-    <t>Uploads a new document into the application</t>
-  </si>
-  <si>
-    <t>Sprint1</t>
+    <t>FLD_DocumentRegistry_New_Transmittals</t>
+  </si>
+  <si>
+    <t>Creates a new Transmittal by attaching a document from Document Registry List.</t>
+  </si>
+  <si>
+    <t>Sprint2</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -528,7 +531,9 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Marked all tests for execution Including upload document test
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/DOCS Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/DOCS Suite.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FluidTX_MayWS\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TCID</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>FLD_CreateNewDocument</t>
@@ -79,7 +73,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -505,16 +498,16 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="73.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -548,7 +541,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
@@ -566,18 +559,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -588,9 +579,7 @@
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>